<commit_message>
sữa thời gian ngừng mấy
</commit_message>
<xml_diff>
--- a/TaiLieu/Phân tích công thức báo cáo tuần và ngày Wahl.xlsx
+++ b/TaiLieu/Phân tích công thức báo cáo tuần và ngày Wahl.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\truon\Documents\Zalo Received Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\01.SmarTrack\TaiLieu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0074D1A-CB7E-41A3-BF69-2D8C43F9AEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789CEBDB-2BA3-44A0-B070-8960AFE435A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="118">
   <si>
     <t>Công thức</t>
   </si>
@@ -327,10 +327,67 @@
     <t>Warmup</t>
   </si>
   <si>
-    <t xml:space="preserve">(SUM(StartTime - EndTime) / 60) / AvailableRunningTime </t>
-  </si>
-  <si>
     <t>Lưu ý</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tóm tắt                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan (pcs)                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual (pcs)                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scrap (pcs)                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">% Scrap                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WarmUp                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minutes of unplanned downtime </t>
+  </si>
+  <si>
+    <t xml:space="preserve">No. of planned downtime       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minutes of planned downtime   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">No. of Changeover             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minutes of Changeover         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total down time (Min)         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OEE (%)                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available running time (Hr)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runing time (Hr)              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilization (%)               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">StandardLabor (Hr)            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ActualLabor (Hr)              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">((MAX(Endtime) - MIN(Start)-plan) / 60 / AvailableRunningTime </t>
   </si>
 </sst>
 </file>
@@ -607,43 +664,53 @@
     <xf numFmtId="4" fontId="4" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -661,52 +728,42 @@
     <xf numFmtId="4" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -988,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK24"/>
+  <dimension ref="A1:AK47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="E20" sqref="E20:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1000,8 +1057,9 @@
     <col min="2" max="3" width="10.7109375" style="6" customWidth="1"/>
     <col min="4" max="4" width="40.42578125" style="6" customWidth="1"/>
     <col min="5" max="6" width="10.7109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="43.7109375" style="7" customWidth="1"/>
-    <col min="8" max="13" width="10.7109375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="40.42578125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" style="8" customWidth="1"/>
+    <col min="9" max="13" width="10.7109375" style="8" customWidth="1"/>
     <col min="14" max="15" width="10.7109375" style="7" customWidth="1"/>
     <col min="16" max="32" width="10.7109375" style="8" customWidth="1"/>
     <col min="33" max="34" width="10.7109375" style="9" customWidth="1"/>
@@ -1014,196 +1072,196 @@
       <c r="A1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="30" t="s">
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
       <c r="H1" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="27" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
     </row>
     <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="32" t="s">
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="34"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="38"/>
     </row>
     <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="27" t="s">
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
     </row>
     <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="27" t="s">
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
     </row>
     <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
     </row>
     <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
     </row>
     <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
     </row>
     <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
     </row>
     <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
     </row>
     <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
     </row>
     <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
     </row>
     <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
     </row>
     <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
@@ -1212,11 +1270,11 @@
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="22"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="45"/>
     </row>
     <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
@@ -1225,150 +1283,307 @@
       <c r="B16" s="13"/>
       <c r="C16" s="15"/>
       <c r="D16" s="16"/>
-      <c r="E16" s="23" t="s">
+      <c r="E16" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="24"/>
-      <c r="G16" s="25"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="48"/>
     </row>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="17" t="s">
+      <c r="B17" s="39"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="18"/>
-      <c r="G17" s="19"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="44"/>
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="17" t="s">
+      <c r="B18" s="39"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="19"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="44"/>
     </row>
     <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="26" t="s">
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
     </row>
     <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="27" t="s">
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
     </row>
     <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="27" t="s">
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
     </row>
     <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
     </row>
     <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="27" t="s">
+      <c r="B23" s="31"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
     </row>
     <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="27" t="s">
+      <c r="B24" s="31"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="5">
+        <v>44669</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="8">
+        <v>324454.26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" s="8">
+        <v>306764</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B31" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" s="6">
+        <v>418.68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" s="6">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" s="6">
+        <v>85.18</v>
+      </c>
+      <c r="D35" s="8">
+        <f>B35+B37</f>
+        <v>2792.31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" s="6">
+        <v>21</v>
+      </c>
+      <c r="D36" s="6">
+        <f>D35/60</f>
+        <v>46.538499999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B37" s="8">
+        <v>2707.13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="6">
+        <v>11.52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B41" s="8">
+        <v>2792.32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B42" s="6">
+        <v>103.07</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" s="6">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B44" s="6">
+        <v>313.45999999999998</v>
+      </c>
+      <c r="D44" s="6">
+        <f>B43-D36</f>
+        <v>313.4615</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B45" s="6">
+        <v>79.14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" s="6">
+        <v>109.45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B47" s="6">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B20:D20"/>
@@ -1381,14 +1596,34 @@
     <mergeCell ref="E19:G19"/>
     <mergeCell ref="E20:G20"/>
     <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E15:G15"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -1437,10 +1672,10 @@
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="37"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="19"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1457,372 +1692,373 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="37"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="37"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="38" t="s">
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="I4" s="40" t="s">
+      <c r="I4" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="J4" s="41"/>
+      <c r="J4" s="22"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="44">
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="24">
         <v>8</v>
       </c>
-      <c r="I5" s="40"/>
-      <c r="J5" s="41"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="22"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="46">
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="26">
         <v>16.899999999999999</v>
       </c>
-      <c r="I6" s="40"/>
-      <c r="J6" s="41"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="50">
+      <c r="B7" s="50"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="27">
         <f>1704</f>
         <v>1704</v>
       </c>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="46">
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="26">
         <v>4816</v>
       </c>
-      <c r="I8" s="40"/>
-      <c r="J8" s="41"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="46">
+      <c r="B9" s="50"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="26">
         <v>0</v>
       </c>
-      <c r="I9" s="40"/>
-      <c r="J9" s="41"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="22"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="46">
+      <c r="B10" s="50"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="26">
         <v>4816</v>
       </c>
-      <c r="I10" s="40"/>
-      <c r="J10" s="41"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="22"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="46">
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="26">
         <f>H9/H10</f>
         <v>0</v>
       </c>
-      <c r="I11" s="40" t="s">
+      <c r="I11" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="J11" s="41"/>
+      <c r="J11" s="22"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="46">
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="26">
         <f>H8-H9</f>
         <v>4816</v>
       </c>
-      <c r="I12" s="40" t="s">
+      <c r="I12" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="J12" s="41"/>
+      <c r="J12" s="22"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="46">
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="26">
         <f>H14*H16</f>
         <v>8055.3759999999993</v>
       </c>
-      <c r="I13" s="40" t="s">
+      <c r="I13" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="J13" s="41"/>
+      <c r="J13" s="22"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="46">
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="26">
         <v>283.64</v>
       </c>
-      <c r="I14" s="51" t="s">
+      <c r="I14" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="J14" s="51" t="s">
+      <c r="J14" s="28" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="46">
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="26">
         <v>205.74</v>
       </c>
-      <c r="I15" s="40" t="s">
+      <c r="I15" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="J15" s="41"/>
+      <c r="J15" s="22"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="46">
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="26">
         <f>H7 / 60</f>
         <v>28.4</v>
       </c>
-      <c r="I16" s="40" t="s">
+      <c r="I16" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="J16" s="41"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="52" t="s">
+      <c r="A17" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="53">
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="30">
         <f xml:space="preserve"> H15 / H14</f>
         <v>0.72535608517839523</v>
       </c>
-      <c r="I17" s="40" t="s">
+      <c r="I17" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="J17" s="41"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="52" t="s">
+      <c r="A18" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="53">
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="30">
         <f>(H8/H15)/H16</f>
         <v>0.82423186929489833</v>
       </c>
-      <c r="I18" s="40" t="s">
+      <c r="I18" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="J18" s="41"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="46">
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="26">
         <f>(H15 * 60) / (H8/H5)</f>
         <v>20.505647840531562</v>
       </c>
-      <c r="I19" s="40" t="s">
+      <c r="I19" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="J19" s="41"/>
+      <c r="J19" s="22"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="52" t="s">
+      <c r="A20" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="53">
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="30">
         <f xml:space="preserve"> (H8-H9) / H8</f>
         <v>1</v>
       </c>
-      <c r="I20" s="40" t="s">
+      <c r="I20" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="J20" s="41"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="52" t="s">
+      <c r="A21" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="53">
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="30">
         <f xml:space="preserve"> H17*H18*H20</f>
         <v>0.59786160199101823</v>
       </c>
-      <c r="I21" s="40" t="s">
+      <c r="I21" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="J21" s="41"/>
+      <c r="J21" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
     <mergeCell ref="B21:G21"/>
     <mergeCell ref="B10:G10"/>
     <mergeCell ref="B11:G11"/>
@@ -1830,12 +2066,11 @@
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="B14:G14"/>
     <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
đêm HMI về nhà test
</commit_message>
<xml_diff>
--- a/TaiLieu/Phân tích công thức báo cáo tuần và ngày Wahl.xlsx
+++ b/TaiLieu/Phân tích công thức báo cáo tuần và ngày Wahl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\01.SmarTrack\TaiLieu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0A4064-B62C-4D08-A03B-123F0A9D7B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBA3EB9-5A77-416A-B90D-B63278E37045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -387,7 +387,7 @@
     <t xml:space="preserve">ActualLabor (Hr)              </t>
   </si>
   <si>
-    <t xml:space="preserve">((MAX(Endtime) - MIN(Start)-plan) / 60 / AvailableRunningTime </t>
+    <t xml:space="preserve">((MAX(Endtime) - MIN(Start)-plan) / AvailableRunningTime </t>
   </si>
 </sst>
 </file>
@@ -704,43 +704,13 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="4" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -758,13 +728,43 @@
     <xf numFmtId="4" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1048,7 +1048,7 @@
   <dimension ref="A1:AK47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1057,7 +1057,7 @@
     <col min="2" max="3" width="10.7109375" style="6" customWidth="1"/>
     <col min="4" max="4" width="40.42578125" style="6" customWidth="1"/>
     <col min="5" max="6" width="10.7109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="40.42578125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="38.5703125" style="7" customWidth="1"/>
     <col min="8" max="8" width="32.28515625" style="8" customWidth="1"/>
     <col min="9" max="13" width="10.7109375" style="8" customWidth="1"/>
     <col min="14" max="15" width="10.7109375" style="7" customWidth="1"/>
@@ -1072,16 +1072,16 @@
       <c r="A1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="44" t="s">
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
       <c r="H1" s="8" t="s">
         <v>97</v>
       </c>
@@ -1090,178 +1090,178 @@
       <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="31" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
     </row>
     <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="46" t="s">
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="47"/>
-      <c r="G3" s="48"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="38"/>
     </row>
     <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="31" t="s">
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
     </row>
     <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="31" t="s">
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
     </row>
     <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
     </row>
     <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
     </row>
     <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
     </row>
     <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
     </row>
     <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
     </row>
     <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
     </row>
     <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
     </row>
     <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
     </row>
     <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
@@ -1270,11 +1270,11 @@
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="36"/>
-      <c r="G15" s="37"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="42"/>
     </row>
     <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
@@ -1283,121 +1283,121 @@
       <c r="B16" s="13"/>
       <c r="C16" s="15"/>
       <c r="D16" s="16"/>
-      <c r="E16" s="38" t="s">
+      <c r="E16" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="39"/>
-      <c r="G16" s="40"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="48"/>
     </row>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="32" t="s">
+      <c r="B17" s="39"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="33"/>
-      <c r="G17" s="34"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="45"/>
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="35"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="32" t="s">
+      <c r="B18" s="39"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="F18" s="33"/>
-      <c r="G18" s="34"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="45"/>
     </row>
     <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="43" t="s">
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
     </row>
     <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="41" t="s">
+      <c r="B20" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="31" t="s">
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
     </row>
     <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="31" t="s">
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
     </row>
     <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="41"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="31" t="s">
+      <c r="B22" s="31"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
     </row>
     <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="41"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="31" t="s">
+      <c r="B23" s="31"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
     </row>
     <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="41"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="31" t="s">
+      <c r="B24" s="31"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
@@ -1578,6 +1578,36 @@
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B24:D24"/>
@@ -1594,36 +1624,6 @@
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -1707,14 +1707,14 @@
       <c r="A4" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
       <c r="H4" s="20" t="s">
         <v>62</v>
       </c>
@@ -1727,12 +1727,12 @@
       <c r="A5" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="53"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
       <c r="H5" s="24">
         <v>8</v>
       </c>
@@ -1743,12 +1743,12 @@
       <c r="A6" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="53"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
       <c r="H6" s="26">
         <v>16.899999999999999</v>
       </c>
@@ -1759,12 +1759,12 @@
       <c r="A7" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="51"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="52"/>
       <c r="H7" s="27">
         <f>1704</f>
         <v>1704</v>
@@ -1776,12 +1776,12 @@
       <c r="A8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
       <c r="H8" s="26">
         <v>4816</v>
       </c>
@@ -1792,12 +1792,12 @@
       <c r="A9" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="49"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="51"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="52"/>
       <c r="H9" s="26">
         <v>0</v>
       </c>
@@ -1808,12 +1808,12 @@
       <c r="A10" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="51"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="52"/>
       <c r="H10" s="26">
         <v>4816</v>
       </c>
@@ -1824,14 +1824,14 @@
       <c r="A11" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
       <c r="H11" s="26">
         <f>H9/H10</f>
         <v>0</v>
@@ -1845,14 +1845,14 @@
       <c r="A12" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
       <c r="H12" s="26">
         <f>H8-H9</f>
         <v>4816</v>
@@ -1866,14 +1866,14 @@
       <c r="A13" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
       <c r="H13" s="26">
         <f>H14*H16</f>
         <v>8055.3759999999993</v>
@@ -1887,14 +1887,14 @@
       <c r="A14" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="53" t="s">
+      <c r="B14" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
       <c r="H14" s="26">
         <v>283.64</v>
       </c>
@@ -1909,14 +1909,14 @@
       <c r="A15" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
       <c r="H15" s="26">
         <v>205.74</v>
       </c>
@@ -1929,14 +1929,14 @@
       <c r="A16" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="53" t="s">
+      <c r="B16" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="53"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
       <c r="H16" s="26">
         <f>H7 / 60</f>
         <v>28.4</v>
@@ -1950,14 +1950,14 @@
       <c r="A17" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
       <c r="H17" s="30">
         <f xml:space="preserve"> H15 / H14</f>
         <v>0.72535608517839523</v>
@@ -1971,14 +1971,14 @@
       <c r="A18" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="53" t="s">
+      <c r="B18" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
       <c r="H18" s="30">
         <f>(H8/H15)/H16</f>
         <v>0.82423186929489833</v>
@@ -1992,14 +1992,14 @@
       <c r="A19" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="53" t="s">
+      <c r="B19" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="53"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
       <c r="H19" s="26">
         <f>(H15 * 60) / (H8/H5)</f>
         <v>20.505647840531562</v>
@@ -2013,14 +2013,14 @@
       <c r="A20" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B20" s="53" t="s">
+      <c r="B20" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
       <c r="H20" s="30">
         <f xml:space="preserve"> (H8-H9) / H8</f>
         <v>1</v>
@@ -2034,14 +2034,14 @@
       <c r="A21" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="53" t="s">
+      <c r="B21" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="53"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
       <c r="H21" s="30">
         <f xml:space="preserve"> H17*H18*H20</f>
         <v>0.59786160199101823</v>
@@ -2053,6 +2053,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
     <mergeCell ref="B21:G21"/>
     <mergeCell ref="B10:G10"/>
     <mergeCell ref="B11:G11"/>
@@ -2065,12 +2071,6 @@
     <mergeCell ref="B18:G18"/>
     <mergeCell ref="B19:G19"/>
     <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>